<commit_message>
Updating Mental Health Ontology mapping to LSRs.xlsx
</commit_message>
<xml_diff>
--- a/Mapping to LSRs/Mental Health Ontology mapping to LSRs.xlsx
+++ b/Mapping to LSRs/Mental Health Ontology mapping to LSRs.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,47 +427,47 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>LSR no.</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Extraction sheet dimension</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Variable to extract</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Categories</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Class ID</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Class  label</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Class definition</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Parent class</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Ontology spreadsheet</t>
         </is>
@@ -471,7 +476,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -518,7 +523,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -5194,7 +5199,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Name of arm (e.g., exercise only, exercise + psychotherapy)</t>
+          <t>Name of arm (e.g., exercise only, exercise   psychotherapy)</t>
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
@@ -15916,7 +15921,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t xml:space="preserve">b is a specifically dependent continuant = Def. b is a continuant &amp; there is some independent continuant c which is not a spatial region and which is such that b s-depends_on c at every time t during the course of b�s existence. </t>
+          <t xml:space="preserve">b is a specifically dependent continuant = Def. b is a continuant and there is some independent continuant c which is not a spatial region and which is such that b s-depends_on c at every time t during the course of b�s existence. </t>
         </is>
       </c>
       <c r="H358" t="inlineStr">

</xml_diff>

<commit_message>
Update Mental Health Ontology mapping to LSRs.xlsx
</commit_message>
<xml_diff>
--- a/Mapping to LSRs/Mental Health Ontology mapping to LSRs.xlsx
+++ b/Mapping to LSRs/Mental Health Ontology mapping to LSRs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Documents/GitHub/mental-health-ontology/Mapping to LSRs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_0A1D409F55EAD9D689F7D2524C5ED87656C94087" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{240E5EDC-B384-4C3B-91EA-94410EC9C48D}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_0A1D409F55EAD9D689F7D2524C5ED87656C94087" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75854011-7D32-4075-9E4E-E40FAF358ED3}"/>
   <bookViews>
-    <workbookView xWindow="42225" yWindow="2520" windowWidth="13845" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30000" yWindow="720" windowWidth="16425" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="1487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="1487">
   <si>
     <t>LSR no.</t>
   </si>
@@ -4585,7 +4585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4622,18 +4622,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4939,7 +4938,7 @@
   <dimension ref="A1:M524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4983,11 +4982,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C2" s="15" t="s">
+    <row r="2" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -5008,83 +5007,83 @@
       <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="15"/>
+      <c r="L2" s="14"/>
       <c r="M2" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="17" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>1335</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>16</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="17" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>1336</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>71</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="15" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -5105,18 +5104,18 @@
       <c r="J5" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="15" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -5125,90 +5124,92 @@
       <c r="F6" s="4" t="s">
         <v>1339</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
+        <v>1331</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>1340</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>1341</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>1342</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="K6" s="14"/>
       <c r="M6" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="19" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>1343</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>1344</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="18" t="s">
         <v>144</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="17" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>151</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="16" t="s">
         <v>144</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="15" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -5229,18 +5230,18 @@
       <c r="J9" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="15" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -5261,18 +5262,18 @@
       <c r="J10" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="15" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -5293,18 +5294,18 @@
       <c r="J11" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="15" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -5325,18 +5326,18 @@
       <c r="J12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="15" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -5357,18 +5358,18 @@
       <c r="J13" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="15" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -5389,18 +5390,18 @@
       <c r="J14" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="15" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -5421,18 +5422,18 @@
       <c r="J15" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="15" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -5453,18 +5454,18 @@
       <c r="J16" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="17" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="15" t="s">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -5485,18 +5486,18 @@
       <c r="J17" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="18" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="15" t="s">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -5517,50 +5518,50 @@
       <c r="J18" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="14" t="s">
         <v>144</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="19" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="19" t="s">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C19" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="19" t="s">
         <v>1358</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>1359</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="18" t="s">
         <v>144</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="20" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="15" t="s">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C20" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -5569,28 +5570,28 @@
       <c r="F20" s="4" t="s">
         <v>1361</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>1362</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="14" t="s">
         <v>1363</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="14" t="s">
         <v>1364</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="14" t="s">
         <v>1365</v>
       </c>
-      <c r="K20" s="15"/>
+      <c r="K20" s="14"/>
       <c r="M20" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="21" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="15" t="s">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -5611,18 +5612,18 @@
       <c r="J21" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="K21" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="22" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="15" t="s">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C22" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -5643,18 +5644,18 @@
       <c r="J22" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="23" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="15" t="s">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C23" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -5669,24 +5670,24 @@
       <c r="H23" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="I23" s="21" t="s">
+      <c r="I23" s="20" t="s">
         <v>1373</v>
       </c>
-      <c r="J23" s="21" t="s">
+      <c r="J23" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="24" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="15" t="s">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C24" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -5701,24 +5702,24 @@
       <c r="H24" s="5" t="s">
         <v>1374</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="20" t="s">
         <v>1375</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K24" s="15" t="s">
+      <c r="K24" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="25" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="15" t="s">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C25" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -5739,18 +5740,18 @@
       <c r="J25" s="5" t="s">
         <v>1380</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="26" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="15" t="s">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C26" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -5765,24 +5766,24 @@
       <c r="H26" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="20" t="s">
         <v>1373</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="27" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="15" t="s">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C27" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -5797,24 +5798,24 @@
       <c r="H27" s="5" t="s">
         <v>1374</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="I27" s="20" t="s">
         <v>1375</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="28" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="15" t="s">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C28" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -5829,24 +5830,24 @@
       <c r="H28" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="J28" s="21" t="s">
+      <c r="J28" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K28" s="15" t="s">
+      <c r="K28" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="29" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="15" t="s">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C29" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -5864,21 +5865,21 @@
       <c r="I29" s="5" t="s">
         <v>1384</v>
       </c>
-      <c r="J29" s="21" t="s">
+      <c r="J29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="K29" s="15" t="s">
+      <c r="K29" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="30" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="15" t="s">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C30" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -5893,24 +5894,24 @@
       <c r="H30" s="5" t="s">
         <v>1385</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="I30" s="20" t="s">
         <v>1386</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="K30" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="31" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="15" t="s">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C31" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -5931,18 +5932,18 @@
       <c r="J31" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="K31" s="15" t="s">
+      <c r="K31" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="32" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="15" t="s">
+    <row r="32" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C32" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -5963,18 +5964,18 @@
       <c r="J32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K32" s="15" t="s">
+      <c r="K32" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="33" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="15" t="s">
+    <row r="33" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C33" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -5995,18 +5996,18 @@
       <c r="J33" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K33" s="15" t="s">
+      <c r="K33" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="34" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="15" t="s">
+    <row r="34" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C34" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -6021,24 +6022,24 @@
       <c r="H34" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I34" s="15" t="s">
+      <c r="I34" s="14" t="s">
         <v>186</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="K34" s="15" t="s">
+      <c r="K34" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="35" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="15" t="s">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C35" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -6053,24 +6054,24 @@
       <c r="H35" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="I35" s="14" t="s">
         <v>220</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="K35" s="15" t="s">
+      <c r="K35" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="36" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="15" t="s">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C36" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -6085,24 +6086,24 @@
       <c r="H36" s="4" t="s">
         <v>1385</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="I36" s="14" t="s">
         <v>1386</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>1050</v>
       </c>
-      <c r="K36" s="15" t="s">
+      <c r="K36" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="37" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="15" t="s">
+    <row r="37" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C37" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -6123,18 +6124,18 @@
       <c r="J37" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="K37" s="15" t="s">
+      <c r="K37" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="38" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="15" t="s">
+    <row r="38" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C38" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E38" s="5" t="s">
@@ -6155,18 +6156,18 @@
       <c r="J38" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="K38" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="39" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="15" t="s">
+    <row r="39" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C39" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -6187,18 +6188,18 @@
       <c r="J39" s="5" t="s">
         <v>1380</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="K39" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="40" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="15" t="s">
+    <row r="40" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C40" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E40" s="5" t="s">
@@ -6213,24 +6214,24 @@
       <c r="H40" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="I40" s="21" t="s">
+      <c r="I40" s="20" t="s">
         <v>1373</v>
       </c>
-      <c r="J40" s="21" t="s">
+      <c r="J40" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="K40" s="15" t="s">
+      <c r="K40" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="41" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C41" s="15" t="s">
+    <row r="41" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C41" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E41" s="5" t="s">
@@ -6251,18 +6252,18 @@
       <c r="J41" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="K41" s="15" t="s">
+      <c r="K41" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="42" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C42" s="15" t="s">
+    <row r="42" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C42" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -6277,24 +6278,24 @@
       <c r="H42" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I42" s="15" t="s">
+      <c r="I42" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="J42" s="21" t="s">
+      <c r="J42" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="K42" s="15" t="s">
+      <c r="K42" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="43" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="15" t="s">
+    <row r="43" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C43" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E43" s="5" t="s">
@@ -6312,21 +6313,21 @@
       <c r="I43" s="5" t="s">
         <v>1384</v>
       </c>
-      <c r="J43" s="21" t="s">
+      <c r="J43" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="K43" s="15" t="s">
+      <c r="K43" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="44" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="15" t="s">
+    <row r="44" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C44" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E44" s="5" t="s">
@@ -6341,24 +6342,24 @@
       <c r="H44" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I44" s="21" t="s">
+      <c r="I44" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K44" s="15" t="s">
+      <c r="K44" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M44" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="45" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="15" t="s">
+    <row r="45" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C45" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E45" s="5" t="s">
@@ -6373,24 +6374,24 @@
       <c r="H45" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I45" s="15" t="s">
+      <c r="I45" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="J45" s="21" t="s">
+      <c r="J45" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K45" s="15" t="s">
+      <c r="K45" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="46" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="15" t="s">
+    <row r="46" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C46" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E46" s="5" t="s">
@@ -6399,7 +6400,7 @@
       <c r="F46" s="4" t="s">
         <v>1402</v>
       </c>
-      <c r="G46" s="15" t="s">
+      <c r="G46" s="14" t="s">
         <v>210</v>
       </c>
       <c r="H46" s="5" t="s">
@@ -6411,18 +6412,18 @@
       <c r="J46" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K46" s="15" t="s">
+      <c r="K46" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M46" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="47" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="15" t="s">
+    <row r="47" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C47" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E47" s="5" t="s">
@@ -6437,24 +6438,24 @@
       <c r="H47" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I47" s="21" t="s">
+      <c r="I47" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J47" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K47" s="15" t="s">
+      <c r="K47" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="48" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="15" t="s">
+    <row r="48" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C48" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E48" s="5" t="s">
@@ -6469,24 +6470,24 @@
       <c r="H48" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I48" s="15" t="s">
+      <c r="I48" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="J48" s="21" t="s">
+      <c r="J48" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K48" s="15" t="s">
+      <c r="K48" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="49" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C49" s="15" t="s">
+    <row r="49" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C49" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E49" s="5" t="s">
@@ -6507,18 +6508,18 @@
       <c r="J49" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="K49" s="15" t="s">
+      <c r="K49" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="50" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C50" s="15" t="s">
+    <row r="50" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C50" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E50" s="5" t="s">
@@ -6533,24 +6534,24 @@
       <c r="H50" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I50" s="21" t="s">
+      <c r="I50" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K50" s="15" t="s">
+      <c r="K50" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M50" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="51" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C51" s="15" t="s">
+    <row r="51" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C51" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E51" s="5" t="s">
@@ -6571,18 +6572,18 @@
       <c r="J51" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K51" s="15" t="s">
+      <c r="K51" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M51" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="52" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C52" s="15" t="s">
+    <row r="52" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C52" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E52" s="5" t="s">
@@ -6597,24 +6598,24 @@
       <c r="H52" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I52" s="15" t="s">
+      <c r="I52" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="J52" s="21" t="s">
+      <c r="J52" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K52" s="15" t="s">
+      <c r="K52" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M52" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="53" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C53" s="15" t="s">
+    <row r="53" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C53" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E53" s="5" t="s">
@@ -6629,24 +6630,24 @@
       <c r="H53" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I53" s="21" t="s">
+      <c r="I53" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K53" s="15" t="s">
+      <c r="K53" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M53" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="54" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="15" t="s">
+    <row r="54" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C54" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E54" s="5" t="s">
@@ -6667,18 +6668,18 @@
       <c r="J54" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="K54" s="15" t="s">
+      <c r="K54" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="55" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C55" s="15" t="s">
+    <row r="55" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C55" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E55" s="5" t="s">
@@ -6699,18 +6700,18 @@
       <c r="J55" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="K55" s="15" t="s">
+      <c r="K55" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M55" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="56" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C56" s="15" t="s">
+    <row r="56" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C56" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E56" s="5" t="s">
@@ -6731,18 +6732,18 @@
       <c r="J56" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K56" s="15" t="s">
+      <c r="K56" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M56" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="57" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C57" s="15" t="s">
+    <row r="57" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C57" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E57" s="5" t="s">
@@ -6763,18 +6764,18 @@
       <c r="J57" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K57" s="15" t="s">
+      <c r="K57" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="58" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="15" t="s">
+    <row r="58" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C58" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -6795,18 +6796,18 @@
       <c r="J58" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K58" s="15" t="s">
+      <c r="K58" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M58" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="59" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="15" t="s">
+    <row r="59" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C59" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E59" s="5" t="s">
@@ -6827,18 +6828,18 @@
       <c r="J59" s="4" t="s">
         <v>1380</v>
       </c>
-      <c r="K59" s="15" t="s">
+      <c r="K59" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="60" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C60" s="15" t="s">
+    <row r="60" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C60" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E60" s="5" t="s">
@@ -6853,24 +6854,24 @@
       <c r="H60" s="5" t="s">
         <v>1374</v>
       </c>
-      <c r="I60" s="21" t="s">
+      <c r="I60" s="20" t="s">
         <v>1375</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K60" s="15" t="s">
+      <c r="K60" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="61" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C61" s="15" t="s">
+    <row r="61" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C61" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E61" s="5" t="s">
@@ -6891,18 +6892,18 @@
       <c r="J61" s="9" t="s">
         <v>541</v>
       </c>
-      <c r="K61" s="15" t="s">
+      <c r="K61" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M61" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="62" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C62" s="15" t="s">
+    <row r="62" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C62" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E62" s="5" t="s">
@@ -6923,18 +6924,18 @@
       <c r="J62" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="K62" s="15" t="s">
+      <c r="K62" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="63" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C63" s="15" t="s">
+    <row r="63" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C63" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -6955,18 +6956,18 @@
       <c r="J63" s="9" t="s">
         <v>1050</v>
       </c>
-      <c r="K63" s="15" t="s">
+      <c r="K63" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="64" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C64" s="15" t="s">
+    <row r="64" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C64" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E64" s="5" t="s">
@@ -6975,30 +6976,30 @@
       <c r="F64" s="4" t="s">
         <v>1422</v>
       </c>
-      <c r="G64" s="21" t="s">
+      <c r="G64" s="20" t="s">
         <v>1163</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="I64" s="15" t="s">
+      <c r="I64" s="14" t="s">
         <v>1164</v>
       </c>
-      <c r="J64" s="21" t="s">
+      <c r="J64" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="K64" s="15" t="s">
+      <c r="K64" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M64" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="65" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C65" s="15" t="s">
+    <row r="65" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C65" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E65" s="5" t="s">
@@ -7019,18 +7020,18 @@
       <c r="J65" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K65" s="15" t="s">
+      <c r="K65" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M65" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="66" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="15" t="s">
+    <row r="66" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C66" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E66" s="5" t="s">
@@ -7039,30 +7040,30 @@
       <c r="F66" s="4" t="s">
         <v>1424</v>
       </c>
-      <c r="G66" s="21" t="s">
+      <c r="G66" s="20" t="s">
         <v>1163</v>
       </c>
       <c r="H66" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="I66" s="15" t="s">
+      <c r="I66" s="14" t="s">
         <v>1164</v>
       </c>
-      <c r="J66" s="21" t="s">
+      <c r="J66" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="K66" s="15" t="s">
+      <c r="K66" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M66" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="67" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C67" s="15" t="s">
+    <row r="67" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C67" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E67" s="5" t="s">
@@ -7083,18 +7084,18 @@
       <c r="J67" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="K67" s="15" t="s">
+      <c r="K67" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M67" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="68" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C68" s="15" t="s">
+    <row r="68" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C68" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -7109,24 +7110,24 @@
       <c r="H68" s="5" t="s">
         <v>1385</v>
       </c>
-      <c r="I68" s="21" t="s">
+      <c r="I68" s="20" t="s">
         <v>1386</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K68" s="15" t="s">
+      <c r="K68" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M68" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="69" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C69" s="15" t="s">
+    <row r="69" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C69" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="15" t="s">
+      <c r="D69" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E69" s="5" t="s">
@@ -7147,18 +7148,18 @@
       <c r="J69" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K69" s="15" t="s">
+      <c r="K69" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M69" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="70" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C70" s="15" t="s">
+    <row r="70" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C70" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E70" s="5" t="s">
@@ -7173,24 +7174,24 @@
       <c r="H70" s="5" t="s">
         <v>1393</v>
       </c>
-      <c r="I70" s="21" t="s">
+      <c r="I70" s="20" t="s">
         <v>1394</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K70" s="15" t="s">
+      <c r="K70" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M70" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="71" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C71" s="15" t="s">
+    <row r="71" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C71" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D71" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E71" s="5" t="s">
@@ -7211,18 +7212,18 @@
       <c r="J71" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K71" s="15" t="s">
+      <c r="K71" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M71" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="72" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C72" s="15" t="s">
+    <row r="72" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C72" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D72" s="15" t="s">
+      <c r="D72" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E72" s="5" t="s">
@@ -7237,24 +7238,24 @@
       <c r="H72" s="5" t="s">
         <v>1393</v>
       </c>
-      <c r="I72" s="21" t="s">
+      <c r="I72" s="20" t="s">
         <v>1394</v>
       </c>
       <c r="J72" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="15" t="s">
+      <c r="K72" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M72" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="73" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C73" s="15" t="s">
+    <row r="73" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C73" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D73" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E73" s="5" t="s">
@@ -7275,18 +7276,18 @@
       <c r="J73" s="4" t="s">
         <v>1380</v>
       </c>
-      <c r="K73" s="15" t="s">
+      <c r="K73" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M73" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="74" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C74" s="15" t="s">
+    <row r="74" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C74" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D74" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E74" s="5" t="s">
@@ -7307,18 +7308,18 @@
       <c r="J74" s="10" t="s">
         <v>541</v>
       </c>
-      <c r="K74" s="15" t="s">
+      <c r="K74" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M74" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="75" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C75" s="15" t="s">
+    <row r="75" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C75" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E75" s="5" t="s">
@@ -7339,18 +7340,18 @@
       <c r="J75" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="K75" s="15" t="s">
+      <c r="K75" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M75" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="76" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C76" s="15" t="s">
+    <row r="76" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C76" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D76" s="15" t="s">
+      <c r="D76" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E76" s="5" t="s">
@@ -7371,18 +7372,18 @@
       <c r="J76" s="9" t="s">
         <v>1050</v>
       </c>
-      <c r="K76" s="15" t="s">
+      <c r="K76" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M76" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="77" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C77" s="15" t="s">
+    <row r="77" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C77" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="15" t="s">
+      <c r="D77" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E77" s="5" t="s">
@@ -7391,30 +7392,30 @@
       <c r="F77" s="4" t="s">
         <v>1432</v>
       </c>
-      <c r="G77" s="21" t="s">
+      <c r="G77" s="20" t="s">
         <v>1163</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="I77" s="15" t="s">
+      <c r="I77" s="14" t="s">
         <v>1164</v>
       </c>
-      <c r="J77" s="21" t="s">
+      <c r="J77" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="K77" s="15" t="s">
+      <c r="K77" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M77" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="78" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C78" s="15" t="s">
+    <row r="78" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C78" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D78" s="15" t="s">
+      <c r="D78" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E78" s="5" t="s">
@@ -7435,18 +7436,18 @@
       <c r="J78" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K78" s="15" t="s">
+      <c r="K78" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M78" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="79" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C79" s="15" t="s">
+    <row r="79" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C79" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D79" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E79" s="5" t="s">
@@ -7461,24 +7462,24 @@
       <c r="H79" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I79" s="21" t="s">
+      <c r="I79" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J79" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K79" s="15" t="s">
+      <c r="K79" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M79" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="80" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C80" s="15" t="s">
+    <row r="80" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C80" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="D80" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E80" s="5" t="s">
@@ -7487,30 +7488,30 @@
       <c r="F80" s="5" t="s">
         <v>1434</v>
       </c>
-      <c r="G80" s="21" t="s">
+      <c r="G80" s="20" t="s">
         <v>1163</v>
       </c>
       <c r="H80" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="I80" s="15" t="s">
+      <c r="I80" s="14" t="s">
         <v>1164</v>
       </c>
-      <c r="J80" s="21" t="s">
+      <c r="J80" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="K80" s="15" t="s">
+      <c r="K80" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M80" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="81" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="15" t="s">
+    <row r="81" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C81" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E81" s="5" t="s">
@@ -7531,18 +7532,18 @@
       <c r="J81" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="K81" s="15" t="s">
+      <c r="K81" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M81" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="82" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C82" s="15" t="s">
+    <row r="82" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C82" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D82" s="15" t="s">
+      <c r="D82" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E82" s="5" t="s">
@@ -7557,24 +7558,24 @@
       <c r="H82" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I82" s="21" t="s">
+      <c r="I82" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J82" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K82" s="15" t="s">
+      <c r="K82" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M82" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="83" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C83" s="15" t="s">
+    <row r="83" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C83" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D83" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E83" s="5" t="s">
@@ -7595,18 +7596,18 @@
       <c r="J83" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K83" s="15" t="s">
+      <c r="K83" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M83" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="84" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C84" s="15" t="s">
+    <row r="84" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C84" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="D84" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E84" s="5" t="s">
@@ -7615,30 +7616,30 @@
       <c r="F84" s="5" t="s">
         <v>1436</v>
       </c>
-      <c r="G84" s="21" t="s">
+      <c r="G84" s="20" t="s">
         <v>1163</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="I84" s="15" t="s">
+      <c r="I84" s="14" t="s">
         <v>1164</v>
       </c>
-      <c r="J84" s="21" t="s">
+      <c r="J84" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K84" s="15" t="s">
+      <c r="K84" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M84" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="85" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C85" s="15" t="s">
+    <row r="85" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C85" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="15" t="s">
+      <c r="D85" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E85" s="5" t="s">
@@ -7653,24 +7654,24 @@
       <c r="H85" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I85" s="21" t="s">
+      <c r="I85" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J85" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K85" s="15" t="s">
+      <c r="K85" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M85" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="86" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C86" s="15" t="s">
+    <row r="86" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C86" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D86" s="15" t="s">
+      <c r="D86" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E86" s="5" t="s">
@@ -7682,27 +7683,27 @@
       <c r="G86" s="5" t="s">
         <v>1331</v>
       </c>
-      <c r="H86" s="15" t="s">
+      <c r="H86" s="14" t="s">
         <v>1411</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>1412</v>
       </c>
-      <c r="J86" s="15" t="s">
+      <c r="J86" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="K86" s="15" t="s">
+      <c r="K86" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M86" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="87" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C87" s="15" t="s">
+    <row r="87" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C87" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="D87" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E87" s="5" t="s">
@@ -7711,30 +7712,30 @@
       <c r="F87" s="5" t="s">
         <v>1438</v>
       </c>
-      <c r="G87" s="21" t="s">
+      <c r="G87" s="20" t="s">
         <v>1163</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="I87" s="15" t="s">
+      <c r="I87" s="14" t="s">
         <v>1164</v>
       </c>
-      <c r="J87" s="21" t="s">
+      <c r="J87" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K87" s="15" t="s">
+      <c r="K87" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M87" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="88" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C88" s="15" t="s">
+    <row r="88" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C88" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D88" s="15" t="s">
+      <c r="D88" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E88" s="5" t="s">
@@ -7749,24 +7750,24 @@
       <c r="H88" s="5" t="s">
         <v>1441</v>
       </c>
-      <c r="I88" s="21" t="s">
+      <c r="I88" s="20" t="s">
         <v>1442</v>
       </c>
-      <c r="J88" s="21" t="s">
+      <c r="J88" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="K88" s="15" t="s">
+      <c r="K88" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M88" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="89" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C89" s="15" t="s">
+    <row r="89" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C89" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="15" t="s">
+      <c r="D89" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E89" s="5" t="s">
@@ -7781,24 +7782,24 @@
       <c r="H89" s="5" t="s">
         <v>1374</v>
       </c>
-      <c r="I89" s="21" t="s">
+      <c r="I89" s="20" t="s">
         <v>1375</v>
       </c>
       <c r="J89" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K89" s="15" t="s">
+      <c r="K89" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M89" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="90" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C90" s="15" t="s">
+    <row r="90" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C90" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D90" s="15" t="s">
+      <c r="D90" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E90" s="5" t="s">
@@ -7813,24 +7814,24 @@
       <c r="H90" s="5" t="s">
         <v>1441</v>
       </c>
-      <c r="I90" s="21" t="s">
+      <c r="I90" s="20" t="s">
         <v>1442</v>
       </c>
-      <c r="J90" s="21" t="s">
+      <c r="J90" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="K90" s="15" t="s">
+      <c r="K90" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M90" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="91" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C91" s="15" t="s">
+    <row r="91" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C91" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D91" s="15" t="s">
+      <c r="D91" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E91" s="5" t="s">
@@ -7851,18 +7852,18 @@
       <c r="J91" s="4" t="s">
         <v>1380</v>
       </c>
-      <c r="K91" s="15" t="s">
+      <c r="K91" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M91" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="92" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C92" s="15" t="s">
+    <row r="92" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C92" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D92" s="15" t="s">
+      <c r="D92" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E92" s="5" t="s">
@@ -7877,24 +7878,24 @@
       <c r="H92" s="5" t="s">
         <v>1374</v>
       </c>
-      <c r="I92" s="21" t="s">
+      <c r="I92" s="20" t="s">
         <v>1375</v>
       </c>
       <c r="J92" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K92" s="15" t="s">
+      <c r="K92" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M92" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="93" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C93" s="15" t="s">
+    <row r="93" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C93" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D93" s="15" t="s">
+      <c r="D93" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E93" s="5" t="s">
@@ -7915,18 +7916,18 @@
       <c r="J93" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="K93" s="15" t="s">
+      <c r="K93" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M93" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="94" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C94" s="15" t="s">
+    <row r="94" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C94" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D94" s="15" t="s">
+      <c r="D94" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E94" s="5" t="s">
@@ -7944,21 +7945,21 @@
       <c r="I94" s="5" t="s">
         <v>1384</v>
       </c>
-      <c r="J94" s="21" t="s">
+      <c r="J94" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="K94" s="15" t="s">
+      <c r="K94" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M94" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="95" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C95" s="15" t="s">
+    <row r="95" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C95" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="D95" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E95" s="5" t="s">
@@ -7973,24 +7974,24 @@
       <c r="H95" s="5" t="s">
         <v>1385</v>
       </c>
-      <c r="I95" s="21" t="s">
+      <c r="I95" s="20" t="s">
         <v>1386</v>
       </c>
       <c r="J95" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K95" s="15" t="s">
+      <c r="K95" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M95" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="96" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C96" s="15" t="s">
+    <row r="96" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C96" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D96" s="15" t="s">
+      <c r="D96" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E96" s="5" t="s">
@@ -7999,7 +8000,7 @@
       <c r="F96" s="5" t="s">
         <v>1448</v>
       </c>
-      <c r="G96" s="21" t="s">
+      <c r="G96" s="20" t="s">
         <v>190</v>
       </c>
       <c r="H96" s="5" t="s">
@@ -8011,18 +8012,18 @@
       <c r="J96" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="K96" s="15" t="s">
+      <c r="K96" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M96" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="97" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C97" s="15" t="s">
+    <row r="97" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C97" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D97" s="15" t="s">
+      <c r="D97" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E97" s="5" t="s">
@@ -8043,18 +8044,18 @@
       <c r="J97" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K97" s="15" t="s">
+      <c r="K97" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M97" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="98" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C98" s="15" t="s">
+    <row r="98" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C98" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D98" s="15" t="s">
+      <c r="D98" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E98" s="5" t="s">
@@ -8069,24 +8070,24 @@
       <c r="H98" s="5" t="s">
         <v>1385</v>
       </c>
-      <c r="I98" s="21" t="s">
+      <c r="I98" s="20" t="s">
         <v>1386</v>
       </c>
       <c r="J98" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K98" s="15" t="s">
+      <c r="K98" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M98" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="99" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C99" s="15" t="s">
+    <row r="99" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C99" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D99" s="15" t="s">
+      <c r="D99" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E99" s="5" t="s">
@@ -8095,7 +8096,7 @@
       <c r="F99" s="5" t="s">
         <v>1450</v>
       </c>
-      <c r="G99" s="21" t="s">
+      <c r="G99" s="20" t="s">
         <v>190</v>
       </c>
       <c r="H99" s="5" t="s">
@@ -8104,21 +8105,21 @@
       <c r="I99" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="J99" s="21" t="s">
+      <c r="J99" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="K99" s="15" t="s">
+      <c r="K99" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M99" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="100" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C100" s="15" t="s">
+    <row r="100" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C100" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D100" s="15" t="s">
+      <c r="D100" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E100" s="5" t="s">
@@ -8139,18 +8140,18 @@
       <c r="J100" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="K100" s="15" t="s">
+      <c r="K100" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M100" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="101" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C101" s="15" t="s">
+    <row r="101" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C101" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D101" s="15" t="s">
+      <c r="D101" s="14" t="s">
         <v>103</v>
       </c>
       <c r="E101" s="5" t="s">
@@ -8165,24 +8166,24 @@
       <c r="H101" s="5" t="s">
         <v>1385</v>
       </c>
-      <c r="I101" s="21" t="s">
+      <c r="I101" s="20" t="s">
         <v>1386</v>
       </c>
       <c r="J101" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K101" s="15" t="s">
+      <c r="K101" s="14" t="s">
         <v>71</v>
       </c>
       <c r="M101" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="102" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C102" s="15" t="s">
+    <row r="102" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C102" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D102" s="15" t="s">
+      <c r="D102" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E102" s="5" t="s">
@@ -8197,24 +8198,24 @@
       <c r="H102" s="5" t="s">
         <v>1441</v>
       </c>
-      <c r="I102" s="21" t="s">
+      <c r="I102" s="20" t="s">
         <v>1442</v>
       </c>
-      <c r="J102" s="21" t="s">
+      <c r="J102" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="K102" s="15" t="s">
+      <c r="K102" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M102" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="103" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C103" s="15" t="s">
+    <row r="103" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C103" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D103" s="15" t="s">
+      <c r="D103" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E103" s="5" t="s">
@@ -8229,24 +8230,24 @@
       <c r="H103" s="5" t="s">
         <v>1393</v>
       </c>
-      <c r="I103" s="21" t="s">
+      <c r="I103" s="20" t="s">
         <v>1394</v>
       </c>
       <c r="J103" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K103" s="15" t="s">
+      <c r="K103" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M103" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="104" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C104" s="15" t="s">
+    <row r="104" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C104" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D104" s="15" t="s">
+      <c r="D104" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E104" s="5" t="s">
@@ -8261,24 +8262,24 @@
       <c r="H104" s="5" t="s">
         <v>1441</v>
       </c>
-      <c r="I104" s="21" t="s">
+      <c r="I104" s="20" t="s">
         <v>1442</v>
       </c>
-      <c r="J104" s="21" t="s">
+      <c r="J104" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="K104" s="15" t="s">
+      <c r="K104" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M104" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="105" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C105" s="15" t="s">
+    <row r="105" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C105" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D105" s="15" t="s">
+      <c r="D105" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E105" s="5" t="s">
@@ -8293,24 +8294,24 @@
       <c r="H105" s="5" t="s">
         <v>1393</v>
       </c>
-      <c r="I105" s="21" t="s">
+      <c r="I105" s="20" t="s">
         <v>1394</v>
       </c>
       <c r="J105" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K105" s="15" t="s">
+      <c r="K105" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M105" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="106" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C106" s="15" t="s">
+    <row r="106" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C106" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D106" s="15" t="s">
+      <c r="D106" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E106" s="5" t="s">
@@ -8331,18 +8332,18 @@
       <c r="J106" s="4" t="s">
         <v>1380</v>
       </c>
-      <c r="K106" s="15" t="s">
+      <c r="K106" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M106" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="107" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C107" s="15" t="s">
+    <row r="107" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C107" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D107" s="15" t="s">
+      <c r="D107" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E107" s="5" t="s">
@@ -8351,7 +8352,7 @@
       <c r="F107" s="5" t="s">
         <v>1456</v>
       </c>
-      <c r="G107" s="21" t="s">
+      <c r="G107" s="20" t="s">
         <v>190</v>
       </c>
       <c r="H107" s="5" t="s">
@@ -8360,21 +8361,21 @@
       <c r="I107" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="J107" s="21" t="s">
+      <c r="J107" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="K107" s="15" t="s">
+      <c r="K107" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M107" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="108" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C108" s="15" t="s">
+    <row r="108" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C108" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D108" s="15" t="s">
+      <c r="D108" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E108" s="5" t="s">
@@ -8392,21 +8393,21 @@
       <c r="I108" s="5" t="s">
         <v>1384</v>
       </c>
-      <c r="J108" s="21" t="s">
+      <c r="J108" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="K108" s="15" t="s">
+      <c r="K108" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M108" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="109" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C109" s="15" t="s">
+    <row r="109" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C109" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D109" s="15" t="s">
+      <c r="D109" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E109" s="5" t="s">
@@ -8421,24 +8422,24 @@
       <c r="H109" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I109" s="21" t="s">
+      <c r="I109" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J109" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K109" s="15" t="s">
+      <c r="K109" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M109" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="110" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C110" s="15" t="s">
+    <row r="110" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C110" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D110" s="15" t="s">
+      <c r="D110" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E110" s="5" t="s">
@@ -8447,7 +8448,7 @@
       <c r="F110" s="5" t="s">
         <v>1458</v>
       </c>
-      <c r="G110" s="21" t="s">
+      <c r="G110" s="20" t="s">
         <v>190</v>
       </c>
       <c r="H110" s="5" t="s">
@@ -8456,21 +8457,21 @@
       <c r="I110" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="J110" s="21" t="s">
+      <c r="J110" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="K110" s="15" t="s">
+      <c r="K110" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M110" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="111" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C111" s="15" t="s">
+    <row r="111" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C111" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D111" s="15" t="s">
+      <c r="D111" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E111" s="5" t="s">
@@ -8491,18 +8492,18 @@
       <c r="J111" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K111" s="15" t="s">
+      <c r="K111" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M111" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="112" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C112" s="15" t="s">
+    <row r="112" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C112" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D112" s="15" t="s">
+      <c r="D112" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E112" s="5" t="s">
@@ -8517,24 +8518,24 @@
       <c r="H112" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="I112" s="21" t="s">
+      <c r="I112" s="20" t="s">
         <v>1400</v>
       </c>
       <c r="J112" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="K112" s="15" t="s">
+      <c r="K112" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M112" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="113" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C113" s="15" t="s">
+    <row r="113" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C113" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D113" s="15" t="s">
+      <c r="D113" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E113" s="5" t="s">
@@ -8555,18 +8556,18 @@
       <c r="J113" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="K113" s="15" t="s">
+      <c r="K113" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M113" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="114" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C114" s="15" t="s">
+    <row r="114" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C114" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D114" s="15" t="s">
+      <c r="D114" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E114" s="5" t="s">
@@ -8587,18 +8588,18 @@
       <c r="J114" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="K114" s="15" t="s">
+      <c r="K114" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M114" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="115" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C115" s="15" t="s">
+    <row r="115" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C115" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D115" s="15" t="s">
+      <c r="D115" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E115" s="5" t="s">
@@ -8619,18 +8620,18 @@
       <c r="J115" s="9" t="s">
         <v>1050</v>
       </c>
-      <c r="K115" s="15" t="s">
+      <c r="K115" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M115" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="116" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C116" s="15" t="s">
+    <row r="116" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C116" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D116" s="15" t="s">
+      <c r="D116" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E116" s="5" t="s">
@@ -8651,18 +8652,18 @@
       <c r="J116" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K116" s="15" t="s">
+      <c r="K116" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M116" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="117" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C117" s="15" t="s">
+    <row r="117" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C117" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D117" s="15" t="s">
+      <c r="D117" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E117" s="5" t="s">
@@ -8683,18 +8684,18 @@
       <c r="J117" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="K117" s="15" t="s">
+      <c r="K117" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M117" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="118" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C118" s="15" t="s">
+    <row r="118" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C118" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D118" s="15" t="s">
+      <c r="D118" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E118" s="5" t="s">
@@ -8715,18 +8716,18 @@
       <c r="J118" s="9" t="s">
         <v>1050</v>
       </c>
-      <c r="K118" s="15" t="s">
+      <c r="K118" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M118" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="119" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C119" s="15" t="s">
+    <row r="119" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C119" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D119" s="15" t="s">
+      <c r="D119" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E119" s="5" t="s">
@@ -8747,18 +8748,18 @@
       <c r="J119" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="K119" s="15" t="s">
+      <c r="K119" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M119" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="120" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C120" s="15" t="s">
+    <row r="120" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C120" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D120" s="15" t="s">
+      <c r="D120" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E120" s="5" t="s">
@@ -8779,18 +8780,18 @@
       <c r="J120" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="K120" s="15" t="s">
+      <c r="K120" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M120" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="121" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C121" s="15" t="s">
+    <row r="121" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C121" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D121" s="15" t="s">
+      <c r="D121" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E121" s="5" t="s">
@@ -8811,18 +8812,18 @@
       <c r="J121" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="K121" s="15" t="s">
+      <c r="K121" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M121" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="122" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C122" s="15" t="s">
+    <row r="122" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C122" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D122" s="15" t="s">
+      <c r="D122" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E122" s="5" t="s">
@@ -8843,18 +8844,18 @@
       <c r="J122" s="5" t="s">
         <v>1342</v>
       </c>
-      <c r="K122" s="15" t="s">
+      <c r="K122" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M122" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="123" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C123" s="15" t="s">
+    <row r="123" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C123" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D123" s="15" t="s">
+      <c r="D123" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E123" s="5" t="s">
@@ -8875,18 +8876,18 @@
       <c r="J123" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="K123" s="15" t="s">
+      <c r="K123" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M123" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="124" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C124" s="15" t="s">
+    <row r="124" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C124" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D124" s="15" t="s">
+      <c r="D124" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E124" s="5" t="s">
@@ -8907,18 +8908,18 @@
       <c r="J124" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="K124" s="15" t="s">
+      <c r="K124" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M124" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="125" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C125" s="15" t="s">
+    <row r="125" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C125" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D125" s="15" t="s">
+      <c r="D125" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E125" s="5" t="s">
@@ -8939,18 +8940,18 @@
       <c r="J125" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="K125" s="15" t="s">
+      <c r="K125" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M125" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="126" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C126" s="15" t="s">
+    <row r="126" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C126" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D126" s="15" t="s">
+      <c r="D126" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E126" s="5" t="s">
@@ -8971,18 +8972,18 @@
       <c r="J126" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="K126" s="15" t="s">
+      <c r="K126" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M126" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="127" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C127" s="15" t="s">
+    <row r="127" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C127" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D127" s="15" t="s">
+      <c r="D127" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E127" s="5" t="s">
@@ -9003,18 +9004,18 @@
       <c r="J127" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="K127" s="15" t="s">
+      <c r="K127" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M127" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="128" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C128" s="15" t="s">
+    <row r="128" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C128" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D128" s="15" t="s">
+      <c r="D128" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E128" s="5" t="s">
@@ -9035,18 +9036,18 @@
       <c r="J128" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="K128" s="15" t="s">
+      <c r="K128" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M128" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="129" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C129" s="15" t="s">
+    <row r="129" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C129" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D129" s="15" t="s">
+      <c r="D129" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E129" s="5" t="s">
@@ -9067,18 +9068,18 @@
       <c r="J129" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="K129" s="15" t="s">
+      <c r="K129" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M129" s="4" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="130" spans="3:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C130" s="15" t="s">
+    <row r="130" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C130" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D130" s="15" t="s">
+      <c r="D130" s="14" t="s">
         <v>178</v>
       </c>
       <c r="E130" s="5" t="s">
@@ -9099,7 +9100,7 @@
       <c r="J130" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="K130" s="15" t="s">
+      <c r="K130" s="14" t="s">
         <v>137</v>
       </c>
       <c r="M130" s="4" t="s">

</xml_diff>